<commit_message>
Before making Mode into a buidler
</commit_message>
<xml_diff>
--- a/Results/The one in the DB/Hybrid performance per classifier.xlsx
+++ b/Results/The one in the DB/Hybrid performance per classifier.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\NetBeansProjects\formatKDDArff\Results\The one in the DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="12">
   <si>
     <t>J48</t>
   </si>
@@ -414,7 +414,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,6 +887,9 @@
       <c r="A16" t="s">
         <v>0</v>
       </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
       <c r="C16">
         <f>(C2*C9)/100</f>
         <v>96.884874575891985</v>
@@ -910,6 +913,9 @@
       <c r="I16" t="s">
         <v>0</v>
       </c>
+      <c r="J16" t="s">
+        <v>11</v>
+      </c>
       <c r="K16">
         <f>(K2*K9)/100</f>
         <v>78.093443735891995</v>
@@ -935,6 +941,9 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
       <c r="C17">
         <f t="shared" ref="C17:G17" si="2">(C3*C10)/100</f>
         <v>95.858745585404506</v>
@@ -958,6 +967,9 @@
       <c r="I17" t="s">
         <v>2</v>
       </c>
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
       <c r="K17">
         <f t="shared" ref="K17:O17" si="3">(K3*K10)/100</f>
         <v>77.703708332607505</v>
@@ -983,6 +995,9 @@
       <c r="A18" t="s">
         <v>3</v>
       </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
       <c r="C18">
         <f t="shared" ref="C18:G18" si="4">(C4*C11)/100</f>
         <v>51.554211891052503</v>
@@ -1006,6 +1021,9 @@
       <c r="I18" t="s">
         <v>3</v>
       </c>
+      <c r="J18" t="s">
+        <v>11</v>
+      </c>
       <c r="K18">
         <f t="shared" ref="K18:O18" si="5">(K4*K11)/100</f>
         <v>41.841371177262999</v>
@@ -1031,6 +1049,9 @@
       <c r="A19" t="s">
         <v>4</v>
       </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
       <c r="C19">
         <f t="shared" ref="C19:G19" si="6">(C5*C12)/100</f>
         <v>97.737267690039985</v>
@@ -1054,6 +1075,9 @@
       <c r="I19" t="s">
         <v>4</v>
       </c>
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
       <c r="K19">
         <f t="shared" ref="K19:O19" si="7">(K5*K12)/100</f>
         <v>79.980932250220008</v>
@@ -1079,6 +1103,9 @@
       <c r="A20" t="s">
         <v>5</v>
       </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
       <c r="C20">
         <f t="shared" ref="C20:G20" si="8">(C6*C13)/100</f>
         <v>93.207027918939986</v>
@@ -1101,6 +1128,9 @@
       </c>
       <c r="I20" t="s">
         <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>11</v>
       </c>
       <c r="K20">
         <f t="shared" ref="K20:O20" si="9">(K6*K13)/100</f>

</xml_diff>